<commit_message>
refactor based on HW4 solution code
</commit_message>
<xml_diff>
--- a/seattledailydata.xlsx
+++ b/seattledailydata.xlsx
@@ -838,7 +838,7 @@
   <dimension ref="A1:C366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -877,13 +877,37 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>42738</v>
+      </c>
+      <c r="B4">
+        <v>56.75</v>
+      </c>
+      <c r="C4">
+        <v>-1.016666667</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>42739</v>
+      </c>
+      <c r="B5">
+        <v>51.666666669999998</v>
+      </c>
+      <c r="C5">
+        <v>-0.52500000000000002</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>42740</v>
+      </c>
+      <c r="B6">
+        <v>70.708333330000002</v>
+      </c>
+      <c r="C6">
+        <v>-2.4708333329999999</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>

</xml_diff>

<commit_message>
added buggy building heat load calculation
</commit_message>
<xml_diff>
--- a/seattledailydata.xlsx
+++ b/seattledailydata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Average of HOURLYRelativeHumidity</t>
   </si>
@@ -28,6 +28,9 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Average of GHI</t>
   </si>
 </sst>
 </file>
@@ -511,9 +514,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -835,15 +839,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C366"/>
+  <dimension ref="A1:D366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D2" sqref="D2:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -853,8 +857,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42736</v>
       </c>
@@ -864,8 +871,11 @@
       <c r="C2">
         <v>1.032432432</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="2">
+        <v>70.583333333333329</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42737</v>
       </c>
@@ -875,8 +885,11 @@
       <c r="C3">
         <v>-0.18333333299999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="2">
+        <v>72.833333333333329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42738</v>
       </c>
@@ -886,8 +899,11 @@
       <c r="C4">
         <v>-1.016666667</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="2">
+        <v>76.166666666666671</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42739</v>
       </c>
@@ -897,8 +913,11 @@
       <c r="C5">
         <v>-0.52500000000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="2">
+        <v>78.916666666666671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42740</v>
       </c>
@@ -908,35 +927,60 @@
       <c r="C6">
         <v>-2.4708333329999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="2">
+        <v>76.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42741</v>
+      </c>
+      <c r="B7">
+        <v>65.92</v>
+      </c>
+      <c r="C7">
+        <v>-1.6479999999999999</v>
+      </c>
+      <c r="D7" s="2">
+        <v>53.291666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42742</v>
+      </c>
+      <c r="B8">
+        <v>49.708333330000002</v>
+      </c>
+      <c r="C8">
+        <v>0.89583333300000001</v>
+      </c>
+      <c r="D8" s="2">
+        <v>23.833333333333332</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>